<commit_message>
Handles errors and more
1. The website now logs the errors and displays oops.html instead
2. Changed alerts link in homepage
3. added SEO
4. technicals.html fix
5. urls of excel files replaced from absolute urls to relative urls
6. Optimized news app
</commit_message>
<xml_diff>
--- a/techniqo/FeedbackData.xlsx
+++ b/techniqo/FeedbackData.xlsx
@@ -390,7 +390,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:A5"/>
+  <dimension ref="A2:A41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -423,7 +423,263 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Excellent app</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Great work</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Good job</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Good job</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Nice work</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Nicely done</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Nicely done</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Good work</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Great work</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Good work</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Good work team</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Good work team</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>GOod</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Good</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Great</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Great</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Great</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Good work on backtesting</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Good work</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Peers food</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Back</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Good job</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>wow</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>nice</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>fod</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ads</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Good job</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>nicely done</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>wow</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>wow</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>technicals</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>asd</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>very good</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>